<commit_message>
Add fixed datasources for st and minor changes to norming
</commit_message>
<xml_diff>
--- a/cohort analysis/out_round/cohort_analysis_notref_st.xlsx
+++ b/cohort analysis/out_round/cohort_analysis_notref_st.xlsx
@@ -918,7 +918,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>135822</v>
+        <v>48663</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3241,7 +3241,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>4.4314</v>
+        <v>12.3683</v>
       </c>
       <c r="C38">
         <v>19.6849</v>
@@ -3360,7 +3360,7 @@
         <v>12.8256</v>
       </c>
       <c r="C39">
-        <v>5.7698</v>
+        <v>16.104</v>
       </c>
       <c r="D39">
         <v>21.8828</v>
@@ -5786,7 +5786,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>135822</v>
+        <v>48663</v>
       </c>
       <c r="C38">
         <v>6984</v>
@@ -13537,7 +13537,7 @@
         <v>100</v>
       </c>
       <c r="C39">
-        <v>5.54</v>
+        <v>15.46</v>
       </c>
       <c r="D39">
         <v>9.52</v>
@@ -15963,7 +15963,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>0.5600000000000001</v>
+        <v>1.56</v>
       </c>
       <c r="C38">
         <v>3.78</v>
@@ -18505,7 +18505,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>4.4314</v>
+        <v>12.3683</v>
       </c>
       <c r="C38">
         <v>33.4137</v>
@@ -23589,7 +23589,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>4.4314</v>
+        <v>12.3683</v>
       </c>
       <c r="C38">
         <v>5.8547</v>
@@ -23708,7 +23708,7 @@
         <v>12.8256</v>
       </c>
       <c r="C39">
-        <v>1.3384</v>
+        <v>3.7357</v>
       </c>
       <c r="D39">
         <v>2.1979</v>

</xml_diff>

<commit_message>
fix st in 1801
</commit_message>
<xml_diff>
--- a/cohort analysis/out_round/cohort_analysis_notref_st.xlsx
+++ b/cohort analysis/out_round/cohort_analysis_notref_st.xlsx
@@ -921,7 +921,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>135823</v>
+        <v>48663</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3255,7 +3255,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>4.4314</v>
+        <v>12.3683</v>
       </c>
       <c r="C38">
         <v>19.6844</v>
@@ -3374,7 +3374,7 @@
         <v>12.8256</v>
       </c>
       <c r="C39">
-        <v>5.7698</v>
+        <v>16.104</v>
       </c>
       <c r="D39">
         <v>21.8822</v>
@@ -3496,7 +3496,7 @@
         <v>17.782</v>
       </c>
       <c r="D40">
-        <v>6.5458</v>
+        <v>18.2699</v>
       </c>
       <c r="E40">
         <v>23.5664</v>
@@ -5922,7 +5922,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>135823</v>
+        <v>48663</v>
       </c>
       <c r="C38">
         <v>7000</v>
@@ -14042,7 +14042,7 @@
         <v>100</v>
       </c>
       <c r="C39">
-        <v>5.55</v>
+        <v>15.48</v>
       </c>
       <c r="D39">
         <v>9.539999999999999</v>
@@ -14164,7 +14164,7 @@
         <v>16.71</v>
       </c>
       <c r="D40">
-        <v>3.18</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="E40">
         <v>7.65</v>
@@ -16590,7 +16590,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>0.5600000000000001</v>
+        <v>1.56</v>
       </c>
       <c r="C38">
         <v>3.77</v>
@@ -19257,7 +19257,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>4.4314</v>
+        <v>12.3683</v>
       </c>
       <c r="C38">
         <v>33.3373</v>
@@ -24591,7 +24591,7 @@
         <v>76</v>
       </c>
       <c r="B38">
-        <v>4.4314</v>
+        <v>12.3683</v>
       </c>
       <c r="C38">
         <v>5.8545</v>
@@ -24710,7 +24710,7 @@
         <v>12.8256</v>
       </c>
       <c r="C39">
-        <v>1.3384</v>
+        <v>3.7357</v>
       </c>
       <c r="D39">
         <v>2.1979</v>
@@ -24832,7 +24832,7 @@
         <v>4.9564</v>
       </c>
       <c r="D40">
-        <v>0.776</v>
+        <v>2.1659</v>
       </c>
       <c r="E40">
         <v>1.6841</v>

</xml_diff>